<commit_message>
file mẫu thí sinh
</commit_message>
<xml_diff>
--- a/backend/core/static/files/file mẫu thí sinh.xlsx
+++ b/backend/core/static/files/file mẫu thí sinh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trong\Documents\fpt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EBC75C-9EC9-44D5-BEFD-F47FC700B52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6EADF6-3F5A-49C7-8CBE-B8299C107097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="199">
   <si>
     <t>STT</t>
   </si>
@@ -635,13 +635,19 @@
 - Bắt buộc nhập mã NV và họ tên
 - Thông tin trên bảng là ví dụ, có thể xóa
 - Trước khi import file, hãy xóa lưu ý này</t>
+  </si>
+  <si>
+    <t>imageurl</t>
+  </si>
+  <si>
+    <t>linkanh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -719,6 +725,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -752,7 +767,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -773,15 +788,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -860,21 +866,17 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1093,11 +1095,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,6 +1152,9 @@
       <c r="K1" s="4" t="s">
         <v>193</v>
       </c>
+      <c r="L1" s="4" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="2" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
@@ -1185,12 +1190,14 @@
       <c r="K2" s="16">
         <v>1</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="M2" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="26"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19"/>
@@ -1204,10 +1211,10 @@
       <c r="I3" s="19"/>
       <c r="J3" s="21"/>
       <c r="K3" s="19"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19"/>
@@ -1221,10 +1228,10 @@
       <c r="I4" s="19"/>
       <c r="J4" s="21"/>
       <c r="K4" s="19"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
     </row>
     <row r="5" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
@@ -1238,10 +1245,10 @@
       <c r="I5" s="19"/>
       <c r="J5" s="21"/>
       <c r="K5" s="19"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
     </row>
     <row r="6" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
@@ -1255,10 +1262,10 @@
       <c r="I6" s="19"/>
       <c r="J6" s="21"/>
       <c r="K6" s="19"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
     </row>
     <row r="7" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19"/>
@@ -1272,10 +1279,10 @@
       <c r="I7" s="19"/>
       <c r="J7" s="21"/>
       <c r="K7" s="19"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
     </row>
     <row r="8" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19"/>
@@ -1289,10 +1296,7 @@
       <c r="I8" s="19"/>
       <c r="J8" s="21"/>
       <c r="K8" s="19"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
+      <c r="L8" s="27"/>
     </row>
     <row r="9" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
@@ -1306,10 +1310,7 @@
       <c r="I9" s="19"/>
       <c r="J9" s="21"/>
       <c r="K9" s="19"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
+      <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="19"/>
@@ -1323,6 +1324,7 @@
       <c r="I10" s="19"/>
       <c r="J10" s="21"/>
       <c r="K10" s="19"/>
+      <c r="L10" s="26"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="19"/>
@@ -1336,6 +1338,7 @@
       <c r="I11" s="19"/>
       <c r="J11" s="21"/>
       <c r="K11" s="19"/>
+      <c r="L11" s="26"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
@@ -1349,6 +1352,7 @@
       <c r="I12" s="19"/>
       <c r="J12" s="21"/>
       <c r="K12" s="19"/>
+      <c r="L12" s="26"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
@@ -1362,6 +1366,7 @@
       <c r="I13" s="19"/>
       <c r="J13" s="21"/>
       <c r="K13" s="19"/>
+      <c r="L13" s="26"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
@@ -1375,6 +1380,7 @@
       <c r="I14" s="19"/>
       <c r="J14" s="21"/>
       <c r="K14" s="19"/>
+      <c r="L14" s="26"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
@@ -1388,6 +1394,7 @@
       <c r="I15" s="19"/>
       <c r="J15" s="21"/>
       <c r="K15" s="19"/>
+      <c r="L15" s="26"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="19"/>
@@ -1401,8 +1408,9 @@
       <c r="I16" s="19"/>
       <c r="J16" s="21"/>
       <c r="K16" s="19"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L16" s="26"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="21"/>
@@ -1414,8 +1422,9 @@
       <c r="I17" s="19"/>
       <c r="J17" s="21"/>
       <c r="K17" s="19"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L17" s="26"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="19"/>
       <c r="B18" s="20"/>
       <c r="C18" s="21"/>
@@ -1427,8 +1436,9 @@
       <c r="I18" s="19"/>
       <c r="J18" s="21"/>
       <c r="K18" s="19"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L18" s="26"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
@@ -1440,8 +1450,9 @@
       <c r="I19" s="19"/>
       <c r="J19" s="21"/>
       <c r="K19" s="19"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L19" s="26"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
       <c r="B20" s="20"/>
       <c r="C20" s="21"/>
@@ -1453,8 +1464,9 @@
       <c r="I20" s="19"/>
       <c r="J20" s="21"/>
       <c r="K20" s="19"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20" s="26"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="20"/>
       <c r="C21" s="21"/>
@@ -1466,8 +1478,9 @@
       <c r="I21" s="19"/>
       <c r="J21" s="21"/>
       <c r="K21" s="19"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L21" s="26"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="20"/>
       <c r="C22" s="21"/>
@@ -1479,8 +1492,9 @@
       <c r="I22" s="19"/>
       <c r="J22" s="21"/>
       <c r="K22" s="19"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L22" s="26"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="20"/>
       <c r="C23" s="21"/>
@@ -1492,8 +1506,9 @@
       <c r="I23" s="19"/>
       <c r="J23" s="21"/>
       <c r="K23" s="19"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L23" s="26"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="20"/>
       <c r="C24" s="21"/>
@@ -1505,8 +1520,9 @@
       <c r="I24" s="19"/>
       <c r="J24" s="21"/>
       <c r="K24" s="19"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L24" s="26"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="20"/>
       <c r="C25" s="21"/>
@@ -1518,8 +1534,9 @@
       <c r="I25" s="19"/>
       <c r="J25" s="21"/>
       <c r="K25" s="19"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L25" s="26"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="20"/>
       <c r="C26" s="21"/>
@@ -1531,8 +1548,9 @@
       <c r="I26" s="19"/>
       <c r="J26" s="21"/>
       <c r="K26" s="19"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L26" s="26"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="20"/>
       <c r="C27" s="21"/>
@@ -1544,8 +1562,9 @@
       <c r="I27" s="19"/>
       <c r="J27" s="21"/>
       <c r="K27" s="19"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L27" s="26"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="20"/>
       <c r="C28" s="21"/>
@@ -1557,8 +1576,9 @@
       <c r="I28" s="19"/>
       <c r="J28" s="21"/>
       <c r="K28" s="19"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L28" s="26"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="20"/>
       <c r="C29" s="21"/>
@@ -1570,8 +1590,9 @@
       <c r="I29" s="19"/>
       <c r="J29" s="21"/>
       <c r="K29" s="19"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L29" s="26"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="20"/>
       <c r="C30" s="21"/>
@@ -1583,8 +1604,9 @@
       <c r="I30" s="19"/>
       <c r="J30" s="21"/>
       <c r="K30" s="19"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L30" s="26"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="20"/>
       <c r="C31" s="21"/>
@@ -1596,8 +1618,9 @@
       <c r="I31" s="19"/>
       <c r="J31" s="21"/>
       <c r="K31" s="19"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L31" s="26"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
       <c r="B32" s="20"/>
       <c r="C32" s="21"/>
@@ -1609,8 +1632,9 @@
       <c r="I32" s="19"/>
       <c r="J32" s="21"/>
       <c r="K32" s="19"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L32" s="26"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
       <c r="B33" s="20"/>
       <c r="C33" s="21"/>
@@ -1622,8 +1646,9 @@
       <c r="I33" s="19"/>
       <c r="J33" s="21"/>
       <c r="K33" s="19"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L33" s="26"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
       <c r="B34" s="20"/>
       <c r="C34" s="21"/>
@@ -1635,8 +1660,9 @@
       <c r="I34" s="19"/>
       <c r="J34" s="21"/>
       <c r="K34" s="19"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L34" s="26"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
       <c r="B35" s="20"/>
       <c r="C35" s="21"/>
@@ -1648,8 +1674,9 @@
       <c r="I35" s="19"/>
       <c r="J35" s="21"/>
       <c r="K35" s="19"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L35" s="26"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="19"/>
       <c r="B36" s="20"/>
       <c r="C36" s="21"/>
@@ -1661,8 +1688,9 @@
       <c r="I36" s="19"/>
       <c r="J36" s="21"/>
       <c r="K36" s="19"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L36" s="26"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="19"/>
       <c r="B37" s="20"/>
       <c r="C37" s="21"/>
@@ -1674,8 +1702,9 @@
       <c r="I37" s="19"/>
       <c r="J37" s="21"/>
       <c r="K37" s="19"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L37" s="26"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="19"/>
       <c r="B38" s="20"/>
       <c r="C38" s="21"/>
@@ -1687,8 +1716,9 @@
       <c r="I38" s="19"/>
       <c r="J38" s="21"/>
       <c r="K38" s="19"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L38" s="26"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="20"/>
       <c r="C39" s="21"/>
@@ -1700,8 +1730,9 @@
       <c r="I39" s="19"/>
       <c r="J39" s="21"/>
       <c r="K39" s="19"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L39" s="26"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="19"/>
       <c r="B40" s="20"/>
       <c r="C40" s="21"/>
@@ -1713,8 +1744,9 @@
       <c r="I40" s="19"/>
       <c r="J40" s="21"/>
       <c r="K40" s="19"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L40" s="26"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="19"/>
       <c r="B41" s="20"/>
       <c r="C41" s="21"/>
@@ -1726,8 +1758,9 @@
       <c r="I41" s="19"/>
       <c r="J41" s="21"/>
       <c r="K41" s="19"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L41" s="26"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="19"/>
       <c r="B42" s="20"/>
       <c r="C42" s="21"/>
@@ -1739,8 +1772,9 @@
       <c r="I42" s="19"/>
       <c r="J42" s="21"/>
       <c r="K42" s="19"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L42" s="26"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="19"/>
       <c r="B43" s="20"/>
       <c r="C43" s="21"/>
@@ -1752,8 +1786,9 @@
       <c r="I43" s="19"/>
       <c r="J43" s="21"/>
       <c r="K43" s="19"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L43" s="26"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="19"/>
       <c r="B44" s="20"/>
       <c r="C44" s="21"/>
@@ -1765,8 +1800,9 @@
       <c r="I44" s="19"/>
       <c r="J44" s="21"/>
       <c r="K44" s="19"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L44" s="26"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
       <c r="B45" s="20"/>
       <c r="C45" s="21"/>
@@ -1778,8 +1814,9 @@
       <c r="I45" s="19"/>
       <c r="J45" s="21"/>
       <c r="K45" s="19"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L45" s="26"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="19"/>
       <c r="B46" s="20"/>
       <c r="C46" s="21"/>
@@ -1791,8 +1828,9 @@
       <c r="I46" s="19"/>
       <c r="J46" s="21"/>
       <c r="K46" s="19"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L46" s="26"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="19"/>
       <c r="B47" s="20"/>
       <c r="C47" s="21"/>
@@ -1804,8 +1842,9 @@
       <c r="I47" s="19"/>
       <c r="J47" s="21"/>
       <c r="K47" s="19"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L47" s="26"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="19"/>
       <c r="B48" s="20"/>
       <c r="C48" s="21"/>
@@ -1817,8 +1856,9 @@
       <c r="I48" s="19"/>
       <c r="J48" s="21"/>
       <c r="K48" s="19"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L48" s="26"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="19"/>
       <c r="B49" s="20"/>
       <c r="C49" s="21"/>
@@ -1830,8 +1870,9 @@
       <c r="I49" s="19"/>
       <c r="J49" s="21"/>
       <c r="K49" s="19"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L49" s="26"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="19"/>
       <c r="B50" s="20"/>
       <c r="C50" s="21"/>
@@ -1843,8 +1884,9 @@
       <c r="I50" s="19"/>
       <c r="J50" s="21"/>
       <c r="K50" s="19"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L50" s="26"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="19"/>
       <c r="B51" s="20"/>
       <c r="C51" s="21"/>
@@ -1856,8 +1898,9 @@
       <c r="I51" s="19"/>
       <c r="J51" s="21"/>
       <c r="K51" s="19"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L51" s="26"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="19"/>
       <c r="B52" s="20"/>
       <c r="C52" s="21"/>
@@ -1869,8 +1912,9 @@
       <c r="I52" s="19"/>
       <c r="J52" s="21"/>
       <c r="K52" s="19"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L52" s="26"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="19"/>
       <c r="B53" s="20"/>
       <c r="C53" s="21"/>
@@ -1882,8 +1926,9 @@
       <c r="I53" s="19"/>
       <c r="J53" s="21"/>
       <c r="K53" s="19"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L53" s="26"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="19"/>
       <c r="B54" s="20"/>
       <c r="C54" s="21"/>
@@ -1895,8 +1940,9 @@
       <c r="I54" s="19"/>
       <c r="J54" s="21"/>
       <c r="K54" s="19"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L54" s="26"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="19"/>
       <c r="B55" s="20"/>
       <c r="C55" s="21"/>
@@ -1908,8 +1954,9 @@
       <c r="I55" s="19"/>
       <c r="J55" s="21"/>
       <c r="K55" s="19"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L55" s="26"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="19"/>
       <c r="B56" s="20"/>
       <c r="C56" s="21"/>
@@ -1921,8 +1968,9 @@
       <c r="I56" s="19"/>
       <c r="J56" s="21"/>
       <c r="K56" s="19"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L56" s="26"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="19"/>
       <c r="B57" s="20"/>
       <c r="C57" s="21"/>
@@ -1934,8 +1982,9 @@
       <c r="I57" s="19"/>
       <c r="J57" s="21"/>
       <c r="K57" s="19"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L57" s="26"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="19"/>
       <c r="B58" s="20"/>
       <c r="C58" s="21"/>
@@ -1947,8 +1996,9 @@
       <c r="I58" s="19"/>
       <c r="J58" s="21"/>
       <c r="K58" s="19"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L58" s="26"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="19"/>
       <c r="B59" s="20"/>
       <c r="C59" s="21"/>
@@ -1960,8 +2010,9 @@
       <c r="I59" s="19"/>
       <c r="J59" s="21"/>
       <c r="K59" s="19"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L59" s="26"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="19"/>
       <c r="B60" s="20"/>
       <c r="C60" s="21"/>
@@ -1973,8 +2024,9 @@
       <c r="I60" s="19"/>
       <c r="J60" s="21"/>
       <c r="K60" s="19"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L60" s="26"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="19"/>
       <c r="B61" s="20"/>
       <c r="C61" s="21"/>
@@ -1986,8 +2038,9 @@
       <c r="I61" s="19"/>
       <c r="J61" s="21"/>
       <c r="K61" s="19"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L61" s="26"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="19"/>
       <c r="B62" s="20"/>
       <c r="C62" s="21"/>
@@ -1999,8 +2052,9 @@
       <c r="I62" s="19"/>
       <c r="J62" s="21"/>
       <c r="K62" s="19"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L62" s="26"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="19"/>
       <c r="B63" s="20"/>
       <c r="C63" s="21"/>
@@ -2012,8 +2066,9 @@
       <c r="I63" s="19"/>
       <c r="J63" s="21"/>
       <c r="K63" s="19"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L63" s="26"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="19"/>
       <c r="B64" s="20"/>
       <c r="C64" s="21"/>
@@ -2025,8 +2080,9 @@
       <c r="I64" s="19"/>
       <c r="J64" s="21"/>
       <c r="K64" s="19"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L64" s="26"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="19"/>
       <c r="B65" s="20"/>
       <c r="C65" s="21"/>
@@ -2038,8 +2094,9 @@
       <c r="I65" s="19"/>
       <c r="J65" s="21"/>
       <c r="K65" s="19"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L65" s="26"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="19"/>
       <c r="B66" s="20"/>
       <c r="C66" s="21"/>
@@ -2051,8 +2108,9 @@
       <c r="I66" s="19"/>
       <c r="J66" s="21"/>
       <c r="K66" s="19"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L66" s="26"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="19"/>
       <c r="B67" s="20"/>
       <c r="C67" s="21"/>
@@ -2064,8 +2122,9 @@
       <c r="I67" s="19"/>
       <c r="J67" s="21"/>
       <c r="K67" s="19"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L67" s="26"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="19"/>
       <c r="B68" s="20"/>
       <c r="C68" s="21"/>
@@ -2077,8 +2136,9 @@
       <c r="I68" s="19"/>
       <c r="J68" s="21"/>
       <c r="K68" s="19"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L68" s="26"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="19"/>
       <c r="B69" s="20"/>
       <c r="C69" s="21"/>
@@ -2090,8 +2150,9 @@
       <c r="I69" s="19"/>
       <c r="J69" s="21"/>
       <c r="K69" s="19"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L69" s="26"/>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="19"/>
       <c r="B70" s="20"/>
       <c r="C70" s="21"/>
@@ -2103,8 +2164,9 @@
       <c r="I70" s="19"/>
       <c r="J70" s="21"/>
       <c r="K70" s="19"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L70" s="26"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="19"/>
       <c r="B71" s="20"/>
       <c r="C71" s="21"/>
@@ -2116,8 +2178,9 @@
       <c r="I71" s="19"/>
       <c r="J71" s="21"/>
       <c r="K71" s="19"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L71" s="26"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="19"/>
       <c r="B72" s="20"/>
       <c r="C72" s="21"/>
@@ -2129,8 +2192,9 @@
       <c r="I72" s="19"/>
       <c r="J72" s="21"/>
       <c r="K72" s="19"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L72" s="26"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="19"/>
       <c r="B73" s="20"/>
       <c r="C73" s="21"/>
@@ -2142,8 +2206,9 @@
       <c r="I73" s="19"/>
       <c r="J73" s="21"/>
       <c r="K73" s="19"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L73" s="26"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="19"/>
       <c r="B74" s="20"/>
       <c r="C74" s="21"/>
@@ -2155,8 +2220,9 @@
       <c r="I74" s="19"/>
       <c r="J74" s="21"/>
       <c r="K74" s="19"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L74" s="26"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="19"/>
       <c r="B75" s="20"/>
       <c r="C75" s="21"/>
@@ -2168,8 +2234,9 @@
       <c r="I75" s="19"/>
       <c r="J75" s="21"/>
       <c r="K75" s="19"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L75" s="26"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="19"/>
       <c r="B76" s="20"/>
       <c r="C76" s="21"/>
@@ -2181,8 +2248,9 @@
       <c r="I76" s="19"/>
       <c r="J76" s="21"/>
       <c r="K76" s="19"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L76" s="26"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="19"/>
       <c r="B77" s="20"/>
       <c r="C77" s="21"/>
@@ -2194,8 +2262,9 @@
       <c r="I77" s="19"/>
       <c r="J77" s="21"/>
       <c r="K77" s="19"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L77" s="26"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="19"/>
       <c r="B78" s="20"/>
       <c r="C78" s="21"/>
@@ -2207,8 +2276,9 @@
       <c r="I78" s="19"/>
       <c r="J78" s="21"/>
       <c r="K78" s="19"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L78" s="26"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="19"/>
       <c r="B79" s="20"/>
       <c r="C79" s="21"/>
@@ -2220,8 +2290,9 @@
       <c r="I79" s="19"/>
       <c r="J79" s="21"/>
       <c r="K79" s="19"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L79" s="26"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="19"/>
       <c r="B80" s="20"/>
       <c r="C80" s="21"/>
@@ -2233,8 +2304,9 @@
       <c r="I80" s="19"/>
       <c r="J80" s="21"/>
       <c r="K80" s="19"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L80" s="26"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="19"/>
       <c r="B81" s="20"/>
       <c r="C81" s="21"/>
@@ -2246,8 +2318,9 @@
       <c r="I81" s="19"/>
       <c r="J81" s="21"/>
       <c r="K81" s="19"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L81" s="26"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="19"/>
       <c r="B82" s="20"/>
       <c r="C82" s="21"/>
@@ -2259,8 +2332,9 @@
       <c r="I82" s="19"/>
       <c r="J82" s="21"/>
       <c r="K82" s="19"/>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L82" s="26"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="19"/>
       <c r="B83" s="20"/>
       <c r="C83" s="21"/>
@@ -2272,8 +2346,9 @@
       <c r="I83" s="19"/>
       <c r="J83" s="21"/>
       <c r="K83" s="19"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L83" s="26"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="19"/>
       <c r="B84" s="20"/>
       <c r="C84" s="21"/>
@@ -2285,8 +2360,9 @@
       <c r="I84" s="19"/>
       <c r="J84" s="21"/>
       <c r="K84" s="19"/>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L84" s="26"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="19"/>
       <c r="B85" s="20"/>
       <c r="C85" s="21"/>
@@ -2298,8 +2374,9 @@
       <c r="I85" s="19"/>
       <c r="J85" s="21"/>
       <c r="K85" s="19"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L85" s="26"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="19"/>
       <c r="B86" s="20"/>
       <c r="C86" s="21"/>
@@ -2311,8 +2388,9 @@
       <c r="I86" s="19"/>
       <c r="J86" s="21"/>
       <c r="K86" s="19"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L86" s="26"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="19"/>
       <c r="B87" s="20"/>
       <c r="C87" s="21"/>
@@ -2324,8 +2402,9 @@
       <c r="I87" s="19"/>
       <c r="J87" s="21"/>
       <c r="K87" s="19"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L87" s="26"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="19"/>
       <c r="B88" s="20"/>
       <c r="C88" s="21"/>
@@ -2337,8 +2416,9 @@
       <c r="I88" s="19"/>
       <c r="J88" s="21"/>
       <c r="K88" s="19"/>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L88" s="26"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="19"/>
       <c r="B89" s="20"/>
       <c r="C89" s="21"/>
@@ -2350,8 +2430,9 @@
       <c r="I89" s="19"/>
       <c r="J89" s="21"/>
       <c r="K89" s="19"/>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L89" s="26"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="19"/>
       <c r="B90" s="20"/>
       <c r="C90" s="21"/>
@@ -2363,8 +2444,9 @@
       <c r="I90" s="19"/>
       <c r="J90" s="21"/>
       <c r="K90" s="19"/>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L90" s="26"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="19"/>
       <c r="B91" s="20"/>
       <c r="C91" s="21"/>
@@ -2376,8 +2458,9 @@
       <c r="I91" s="19"/>
       <c r="J91" s="21"/>
       <c r="K91" s="19"/>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L91" s="26"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="19"/>
       <c r="B92" s="20"/>
       <c r="C92" s="21"/>
@@ -2389,8 +2472,9 @@
       <c r="I92" s="19"/>
       <c r="J92" s="21"/>
       <c r="K92" s="19"/>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L92" s="26"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="19"/>
       <c r="B93" s="20"/>
       <c r="C93" s="21"/>
@@ -2402,8 +2486,9 @@
       <c r="I93" s="19"/>
       <c r="J93" s="21"/>
       <c r="K93" s="19"/>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L93" s="26"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="19"/>
       <c r="B94" s="20"/>
       <c r="C94" s="21"/>
@@ -2415,8 +2500,9 @@
       <c r="I94" s="19"/>
       <c r="J94" s="21"/>
       <c r="K94" s="19"/>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L94" s="26"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="19"/>
       <c r="B95" s="20"/>
       <c r="C95" s="21"/>
@@ -2428,8 +2514,9 @@
       <c r="I95" s="19"/>
       <c r="J95" s="21"/>
       <c r="K95" s="19"/>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L95" s="26"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="19"/>
       <c r="B96" s="20"/>
       <c r="C96" s="21"/>
@@ -2441,8 +2528,9 @@
       <c r="I96" s="19"/>
       <c r="J96" s="21"/>
       <c r="K96" s="19"/>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L96" s="26"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="19"/>
       <c r="B97" s="20"/>
       <c r="C97" s="21"/>
@@ -2454,8 +2542,9 @@
       <c r="I97" s="19"/>
       <c r="J97" s="21"/>
       <c r="K97" s="19"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L97" s="26"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="19"/>
       <c r="B98" s="20"/>
       <c r="C98" s="21"/>
@@ -2467,8 +2556,9 @@
       <c r="I98" s="19"/>
       <c r="J98" s="21"/>
       <c r="K98" s="19"/>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L98" s="26"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="19"/>
       <c r="B99" s="20"/>
       <c r="C99" s="21"/>
@@ -2480,8 +2570,9 @@
       <c r="I99" s="19"/>
       <c r="J99" s="21"/>
       <c r="K99" s="19"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L99" s="26"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="19"/>
       <c r="B100" s="20"/>
       <c r="C100" s="21"/>
@@ -2493,8 +2584,9 @@
       <c r="I100" s="19"/>
       <c r="J100" s="21"/>
       <c r="K100" s="19"/>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L100" s="26"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="19"/>
       <c r="B101" s="20"/>
       <c r="C101" s="21"/>
@@ -2506,8 +2598,9 @@
       <c r="I101" s="19"/>
       <c r="J101" s="21"/>
       <c r="K101" s="19"/>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L101" s="26"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="19"/>
       <c r="B102" s="20"/>
       <c r="C102" s="21"/>
@@ -2519,8 +2612,9 @@
       <c r="I102" s="19"/>
       <c r="J102" s="21"/>
       <c r="K102" s="19"/>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L102" s="26"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="19"/>
       <c r="B103" s="20"/>
       <c r="C103" s="21"/>
@@ -2532,8 +2626,9 @@
       <c r="I103" s="19"/>
       <c r="J103" s="21"/>
       <c r="K103" s="19"/>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L103" s="26"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="19"/>
       <c r="B104" s="20"/>
       <c r="C104" s="21"/>
@@ -2545,8 +2640,9 @@
       <c r="I104" s="19"/>
       <c r="J104" s="21"/>
       <c r="K104" s="19"/>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L104" s="26"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="19"/>
       <c r="B105" s="20"/>
       <c r="C105" s="21"/>
@@ -2558,8 +2654,9 @@
       <c r="I105" s="19"/>
       <c r="J105" s="21"/>
       <c r="K105" s="19"/>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L105" s="26"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="19"/>
       <c r="B106" s="20"/>
       <c r="C106" s="21"/>
@@ -2571,8 +2668,9 @@
       <c r="I106" s="19"/>
       <c r="J106" s="21"/>
       <c r="K106" s="19"/>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L106" s="26"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="19"/>
       <c r="B107" s="20"/>
       <c r="C107" s="21"/>
@@ -2584,8 +2682,9 @@
       <c r="I107" s="19"/>
       <c r="J107" s="21"/>
       <c r="K107" s="19"/>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L107" s="26"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="19"/>
       <c r="B108" s="20"/>
       <c r="C108" s="21"/>
@@ -2597,8 +2696,9 @@
       <c r="I108" s="19"/>
       <c r="J108" s="21"/>
       <c r="K108" s="19"/>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L108" s="26"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="19"/>
       <c r="B109" s="20"/>
       <c r="C109" s="21"/>
@@ -2610,8 +2710,9 @@
       <c r="I109" s="19"/>
       <c r="J109" s="21"/>
       <c r="K109" s="19"/>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L109" s="26"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="19"/>
       <c r="B110" s="20"/>
       <c r="C110" s="21"/>
@@ -2623,8 +2724,9 @@
       <c r="I110" s="19"/>
       <c r="J110" s="21"/>
       <c r="K110" s="19"/>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L110" s="26"/>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="19"/>
       <c r="B111" s="22"/>
       <c r="C111" s="21"/>
@@ -2636,8 +2738,9 @@
       <c r="I111" s="19"/>
       <c r="J111" s="21"/>
       <c r="K111" s="19"/>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L111" s="26"/>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C112" s="1"/>
       <c r="J112" s="1"/>
     </row>
@@ -6196,7 +6299,7 @@
   </sheetData>
   <autoFilter ref="A1:K111" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="1">
-    <mergeCell ref="L2:N7"/>
+    <mergeCell ref="M2:O7"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E111" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -7460,6 +7563,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5f59c646-0133-4ff2-ab36-e47ce2a396cc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100609311FA00CB6943B86A396441B40CFD" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b2ccf543faa5f2a8ff63faae27818c13">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5f59c646-0133-4ff2-ab36-e47ce2a396cc" xmlns:ns4="bf5e9f62-897a-483e-ab24-f0319c637264" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7a1fe65e5b3b73499ba5110bd7e4dc8" ns3:_="" ns4:_="">
     <xsd:import namespace="5f59c646-0133-4ff2-ab36-e47ce2a396cc"/>
@@ -7698,24 +7818,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2C75A07-61C3-4D4C-AE1B-1D6ECC18BFA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bf5e9f62-897a-483e-ab24-f0319c637264"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="5f59c646-0133-4ff2-ab36-e47ce2a396cc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5f59c646-0133-4ff2-ab36-e47ce2a396cc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99EEB0A8-C945-4AA6-9479-4363D9276864}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DED879A2-695F-48D2-A57A-AE4203E5B208}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7732,29 +7860,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99EEB0A8-C945-4AA6-9479-4363D9276864}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2C75A07-61C3-4D4C-AE1B-1D6ECC18BFA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bf5e9f62-897a-483e-ab24-f0319c637264"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="5f59c646-0133-4ff2-ab36-e47ce2a396cc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>